<commit_message>
well a lot changed....
</commit_message>
<xml_diff>
--- a/old/strommix_formatiert.xlsx
+++ b/old/strommix_formatiert.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="73">
   <si>
     <t>Kategorie</t>
   </si>
@@ -40,10 +40,13 @@
     <t>Erdgas</t>
   </si>
   <si>
+    <t>Export</t>
+  </si>
+  <si>
     <t>Geothermie</t>
   </si>
   <si>
-    <t>IGNORIEREN</t>
+    <t>Import</t>
   </si>
   <si>
     <t>Import/Export</t>
@@ -70,6 +73,9 @@
     <t>Wasserkraft</t>
   </si>
   <si>
+    <t>Wasserstoff</t>
+  </si>
+  <si>
     <t>Wind</t>
   </si>
   <si>
@@ -130,10 +136,13 @@
     <t>Flüssiggas</t>
   </si>
   <si>
+    <t>Ausfuhr von Elektrizität</t>
+  </si>
+  <si>
     <t>Wärmepumpen (Erd- und Umweltwärme)</t>
   </si>
   <si>
-    <t>Insgesamt</t>
+    <t>Einfuhr von Elektrizität</t>
   </si>
   <si>
     <t>Austauschsaldo</t>
@@ -179,9 +188,6 @@
   </si>
   <si>
     <t>Strom (Elektrokessel)</t>
-  </si>
-  <si>
-    <t>Wasserstoff</t>
   </si>
   <si>
     <t>Wärme</t>
@@ -597,7 +603,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA54"/>
+  <dimension ref="A1:AA55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -692,10 +698,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D2" s="2">
         <v>2926818</v>
@@ -772,10 +778,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
@@ -852,10 +858,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -932,10 +938,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D5" s="2">
         <v>243469</v>
@@ -1012,10 +1018,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D6" s="2">
         <v>30547</v>
@@ -1092,10 +1098,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -1172,10 +1178,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D8" s="2">
         <v>110551</v>
@@ -1252,10 +1258,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D9" s="2">
         <v>201651</v>
@@ -1332,10 +1338,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -1412,10 +1418,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D11" s="2">
         <v>215765</v>
@@ -1492,10 +1498,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D12" s="2">
         <v>11836</v>
@@ -1572,10 +1578,10 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D13" s="2">
         <v>51438</v>
@@ -1652,10 +1658,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D14" s="2">
         <v>41935</v>
@@ -1732,10 +1738,10 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -1812,10 +1818,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D16" s="2">
         <v>1894333</v>
@@ -1892,10 +1898,10 @@
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D17" s="2">
         <v>140544281</v>
@@ -1972,10 +1978,10 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D18" s="2">
         <v>110305</v>
@@ -2052,10 +2058,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D19" s="2">
         <v>39982951</v>
@@ -2132,10 +2138,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D20" s="2">
         <v>159</v>
@@ -2212,90 +2218,90 @@
         <v>8</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D21" s="2">
-        <v>0</v>
+        <v>44463109</v>
       </c>
       <c r="E21" s="2">
-        <v>0</v>
+        <v>52379313</v>
       </c>
       <c r="F21" s="2">
-        <v>0</v>
+        <v>50807677</v>
       </c>
       <c r="G21" s="2">
-        <v>0</v>
+        <v>61427462</v>
       </c>
       <c r="H21" s="2">
-        <v>0</v>
+        <v>65441212</v>
       </c>
       <c r="I21" s="2">
-        <v>0</v>
+        <v>62508209</v>
       </c>
       <c r="J21" s="2">
-        <v>12078</v>
+        <v>61769946</v>
       </c>
       <c r="K21" s="2">
-        <v>9482</v>
+        <v>54132291</v>
       </c>
       <c r="L21" s="2">
-        <v>11858</v>
+        <v>57917220</v>
       </c>
       <c r="M21" s="2">
-        <v>10243</v>
+        <v>54768710</v>
       </c>
       <c r="N21" s="2">
-        <v>0</v>
+        <v>66809995</v>
       </c>
       <c r="O21" s="2">
-        <v>50297</v>
+        <v>71416478</v>
       </c>
       <c r="P21" s="2">
-        <v>52831</v>
+        <v>74321863</v>
       </c>
       <c r="Q21" s="2">
-        <v>91532</v>
+        <v>85290316</v>
       </c>
       <c r="R21" s="2">
-        <v>152650</v>
+        <v>78862663</v>
       </c>
       <c r="S21" s="2">
-        <v>147306</v>
+        <v>80301486</v>
       </c>
       <c r="T21" s="2">
-        <v>0</v>
+        <v>80462299</v>
       </c>
       <c r="U21" s="2">
-        <v>0</v>
+        <v>72792688</v>
       </c>
       <c r="V21" s="2">
-        <v>0</v>
+        <v>66930968</v>
       </c>
       <c r="W21" s="2">
-        <v>0</v>
+        <v>70305524</v>
       </c>
       <c r="X21" s="2">
-        <v>0</v>
+        <v>76586091</v>
       </c>
       <c r="Y21" s="2">
-        <v>0</v>
+        <v>60082790</v>
       </c>
       <c r="Z21" s="2">
-        <v>0</v>
+        <v>55389299</v>
       </c>
     </row>
     <row r="22" spans="1:26">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
@@ -2316,34 +2322,34 @@
         <v>0</v>
       </c>
       <c r="J22" s="2">
-        <v>0</v>
+        <v>12078</v>
       </c>
       <c r="K22" s="2">
-        <v>0</v>
+        <v>9482</v>
       </c>
       <c r="L22" s="2">
-        <v>0</v>
+        <v>11858</v>
       </c>
       <c r="M22" s="2">
-        <v>0</v>
+        <v>10243</v>
       </c>
       <c r="N22" s="2">
         <v>0</v>
       </c>
       <c r="O22" s="2">
-        <v>0</v>
+        <v>50297</v>
       </c>
       <c r="P22" s="2">
-        <v>0</v>
+        <v>52831</v>
       </c>
       <c r="Q22" s="2">
-        <v>0</v>
+        <v>91532</v>
       </c>
       <c r="R22" s="2">
-        <v>0</v>
+        <v>152650</v>
       </c>
       <c r="S22" s="2">
-        <v>0</v>
+        <v>147306</v>
       </c>
       <c r="T22" s="2">
         <v>0</v>
@@ -2372,79 +2378,79 @@
         <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D23" s="2">
-        <v>484044339</v>
+        <v>0</v>
       </c>
       <c r="E23" s="2">
-        <v>498149606</v>
+        <v>0</v>
       </c>
       <c r="F23" s="2">
-        <v>498816964</v>
+        <v>0</v>
       </c>
       <c r="G23" s="2">
-        <v>497513512</v>
+        <v>0</v>
       </c>
       <c r="H23" s="2">
-        <v>504927984</v>
+        <v>0</v>
       </c>
       <c r="I23" s="2">
-        <v>488369371</v>
+        <v>0</v>
       </c>
       <c r="J23" s="2">
-        <v>488581285</v>
+        <v>0</v>
       </c>
       <c r="K23" s="2">
-        <v>446467074</v>
+        <v>0</v>
       </c>
       <c r="L23" s="2">
-        <v>468628740</v>
+        <v>0</v>
       </c>
       <c r="M23" s="2">
-        <v>431182391</v>
+        <v>0</v>
       </c>
       <c r="N23" s="2">
-        <v>435448765</v>
+        <v>0</v>
       </c>
       <c r="O23" s="2">
-        <v>431269663</v>
+        <v>0</v>
       </c>
       <c r="P23" s="2">
-        <v>414426524</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="2">
-        <v>402398137</v>
+        <v>0</v>
       </c>
       <c r="R23" s="2">
-        <v>403201939</v>
+        <v>0</v>
       </c>
       <c r="S23" s="2">
-        <v>378941372</v>
+        <v>0</v>
       </c>
       <c r="T23" s="2">
-        <v>361342016</v>
+        <v>0</v>
       </c>
       <c r="U23" s="2">
-        <v>311088542</v>
+        <v>0</v>
       </c>
       <c r="V23" s="2">
-        <v>270489800</v>
+        <v>0</v>
       </c>
       <c r="W23" s="2">
-        <v>298594508</v>
+        <v>0</v>
       </c>
       <c r="X23" s="2">
-        <v>273144777</v>
+        <v>0</v>
       </c>
       <c r="Y23" s="2">
-        <v>197288057</v>
+        <v>0</v>
       </c>
       <c r="Z23" s="2">
-        <v>179503951</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:26">
@@ -2452,79 +2458,79 @@
         <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D24" s="2">
-        <v>6628002</v>
+        <v>51091111</v>
       </c>
       <c r="E24" s="2">
-        <v>-3269564</v>
+        <v>49109749</v>
       </c>
       <c r="F24" s="2">
-        <v>-2621283</v>
+        <v>48186394</v>
       </c>
       <c r="G24" s="2">
-        <v>-4565171</v>
+        <v>56862291</v>
       </c>
       <c r="H24" s="2">
-        <v>-16977128</v>
+        <v>48464084</v>
       </c>
       <c r="I24" s="2">
-        <v>-16555078</v>
+        <v>45953131</v>
       </c>
       <c r="J24" s="2">
-        <v>-20099477</v>
+        <v>41670469</v>
       </c>
       <c r="K24" s="2">
-        <v>-12272991</v>
+        <v>41859300</v>
       </c>
       <c r="L24" s="2">
-        <v>-14955235</v>
+        <v>42961985</v>
       </c>
       <c r="M24" s="2">
-        <v>-3765750</v>
+        <v>51002960</v>
       </c>
       <c r="N24" s="2">
-        <v>-20541009</v>
+        <v>46268986</v>
       </c>
       <c r="O24" s="2">
-        <v>-32194157</v>
+        <v>39222319</v>
       </c>
       <c r="P24" s="2">
-        <v>-33886908</v>
+        <v>40434954</v>
       </c>
       <c r="Q24" s="2">
-        <v>-48282616</v>
+        <v>37007698</v>
       </c>
       <c r="R24" s="2">
-        <v>-50524820</v>
+        <v>28337841</v>
       </c>
       <c r="S24" s="2">
-        <v>-52459764</v>
+        <v>27842337</v>
       </c>
       <c r="T24" s="2">
-        <v>-48717723</v>
+        <v>31726919</v>
       </c>
       <c r="U24" s="2">
-        <v>-32668719</v>
+        <v>40125396</v>
       </c>
       <c r="V24" s="2">
-        <v>-18880474</v>
+        <v>48046985</v>
       </c>
       <c r="W24" s="2">
-        <v>-18580816</v>
+        <v>51731791</v>
       </c>
       <c r="X24" s="2">
-        <v>-27026898</v>
+        <v>49330582</v>
       </c>
       <c r="Y24" s="2">
-        <v>9175369</v>
+        <v>69306080</v>
       </c>
       <c r="Z24" s="2">
-        <v>26323839</v>
+        <v>81658124</v>
       </c>
     </row>
     <row r="25" spans="1:26">
@@ -2532,120 +2538,120 @@
         <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D25" s="2">
-        <v>3102993</v>
+        <v>6628002</v>
       </c>
       <c r="E25" s="2">
-        <v>3516542</v>
+        <v>-3269564</v>
       </c>
       <c r="F25" s="2">
-        <v>3431558</v>
+        <v>-2621283</v>
       </c>
       <c r="G25" s="2">
-        <v>2743325</v>
+        <v>-4565171</v>
       </c>
       <c r="H25" s="2">
-        <v>2661588</v>
+        <v>-16977128</v>
       </c>
       <c r="I25" s="2">
-        <v>2572847</v>
+        <v>-16555078</v>
       </c>
       <c r="J25" s="2">
-        <v>2280769</v>
+        <v>-20099477</v>
       </c>
       <c r="K25" s="2">
-        <v>1241735</v>
+        <v>-12272991</v>
       </c>
       <c r="L25" s="2">
-        <v>2408477</v>
+        <v>-14955235</v>
       </c>
       <c r="M25" s="2">
-        <v>2329829</v>
+        <v>-3765750</v>
       </c>
       <c r="N25" s="2">
-        <v>0</v>
+        <v>-20541009</v>
       </c>
       <c r="O25" s="2">
-        <v>0</v>
+        <v>-32194157</v>
       </c>
       <c r="P25" s="2">
-        <v>0</v>
+        <v>-33886908</v>
       </c>
       <c r="Q25" s="2">
-        <v>0</v>
+        <v>-48282616</v>
       </c>
       <c r="R25" s="2">
-        <v>0</v>
+        <v>-50524820</v>
       </c>
       <c r="S25" s="2">
-        <v>0</v>
+        <v>-52459764</v>
       </c>
       <c r="T25" s="2">
-        <v>0</v>
+        <v>-48717723</v>
       </c>
       <c r="U25" s="2">
-        <v>0</v>
+        <v>-32668719</v>
       </c>
       <c r="V25" s="2">
-        <v>0</v>
+        <v>-18880474</v>
       </c>
       <c r="W25" s="2">
-        <v>0</v>
+        <v>-18580816</v>
       </c>
       <c r="X25" s="2">
-        <v>0</v>
+        <v>-27026898</v>
       </c>
       <c r="Y25" s="2">
-        <v>0</v>
+        <v>9175369</v>
       </c>
       <c r="Z25" s="2">
-        <v>0</v>
+        <v>26323839</v>
       </c>
     </row>
     <row r="26" spans="1:26">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D26" s="2">
-        <v>44985</v>
+        <v>3102993</v>
       </c>
       <c r="E26" s="2">
-        <v>48905</v>
+        <v>3516542</v>
       </c>
       <c r="F26" s="2">
-        <v>41983</v>
+        <v>3431558</v>
       </c>
       <c r="G26" s="2">
-        <v>42711</v>
+        <v>2743325</v>
       </c>
       <c r="H26" s="2">
-        <v>28802</v>
+        <v>2661588</v>
       </c>
       <c r="I26" s="2">
-        <v>646144</v>
+        <v>2572847</v>
       </c>
       <c r="J26" s="2">
-        <v>515282</v>
+        <v>2280769</v>
       </c>
       <c r="K26" s="2">
-        <v>383720</v>
+        <v>1241735</v>
       </c>
       <c r="L26" s="2">
-        <v>476601</v>
+        <v>2408477</v>
       </c>
       <c r="M26" s="2">
-        <v>403312</v>
+        <v>2329829</v>
       </c>
       <c r="N26" s="2">
         <v>0</v>
@@ -2689,43 +2695,43 @@
     </row>
     <row r="27" spans="1:26">
       <c r="A27" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D27" s="2">
-        <v>244012</v>
+        <v>44985</v>
       </c>
       <c r="E27" s="2">
-        <v>253348</v>
+        <v>48905</v>
       </c>
       <c r="F27" s="2">
-        <v>247225</v>
+        <v>41983</v>
       </c>
       <c r="G27" s="2">
-        <v>253826</v>
+        <v>42711</v>
       </c>
       <c r="H27" s="2">
-        <v>216877</v>
+        <v>28802</v>
       </c>
       <c r="I27" s="2">
-        <v>126382</v>
+        <v>646144</v>
       </c>
       <c r="J27" s="2">
-        <v>24068</v>
+        <v>515282</v>
       </c>
       <c r="K27" s="2">
-        <v>26124</v>
+        <v>383720</v>
       </c>
       <c r="L27" s="2">
-        <v>30103</v>
+        <v>476601</v>
       </c>
       <c r="M27" s="2">
-        <v>28168</v>
+        <v>403312</v>
       </c>
       <c r="N27" s="2">
         <v>0</v>
@@ -2758,7 +2764,7 @@
         <v>0</v>
       </c>
       <c r="X27" s="2">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="Y27" s="2">
         <v>0</v>
@@ -2772,76 +2778,76 @@
         <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D28" s="2">
-        <v>156287021</v>
+        <v>244012</v>
       </c>
       <c r="E28" s="2">
-        <v>156455841</v>
+        <v>253348</v>
       </c>
       <c r="F28" s="2">
-        <v>158378456</v>
+        <v>247225</v>
       </c>
       <c r="G28" s="2">
-        <v>154612295</v>
+        <v>253826</v>
       </c>
       <c r="H28" s="2">
-        <v>158710790</v>
+        <v>216877</v>
       </c>
       <c r="I28" s="2">
-        <v>133229498</v>
+        <v>126382</v>
       </c>
       <c r="J28" s="2">
-        <v>140710087</v>
+        <v>24068</v>
       </c>
       <c r="K28" s="2">
-        <v>127690281</v>
+        <v>26124</v>
       </c>
       <c r="L28" s="2">
-        <v>132970650</v>
+        <v>30103</v>
       </c>
       <c r="M28" s="2">
-        <v>102240624</v>
+        <v>28168</v>
       </c>
       <c r="N28" s="2">
-        <v>94180287</v>
+        <v>0</v>
       </c>
       <c r="O28" s="2">
-        <v>92127247</v>
+        <v>0</v>
       </c>
       <c r="P28" s="2">
-        <v>91800049</v>
+        <v>0</v>
       </c>
       <c r="Q28" s="2">
-        <v>86765007</v>
+        <v>0</v>
       </c>
       <c r="R28" s="2">
-        <v>80038153</v>
+        <v>0</v>
       </c>
       <c r="S28" s="2">
-        <v>72154983</v>
+        <v>0</v>
       </c>
       <c r="T28" s="2">
-        <v>71866451</v>
+        <v>0</v>
       </c>
       <c r="U28" s="2">
-        <v>70992174</v>
+        <v>0</v>
       </c>
       <c r="V28" s="2">
-        <v>60914325</v>
+        <v>0</v>
       </c>
       <c r="W28" s="2">
-        <v>65444269</v>
+        <v>0</v>
       </c>
       <c r="X28" s="2">
-        <v>32765409</v>
+        <v>162</v>
       </c>
       <c r="Y28" s="2">
-        <v>4996402</v>
+        <v>0</v>
       </c>
       <c r="Z28" s="2">
         <v>0</v>
@@ -2852,360 +2858,360 @@
         <v>13</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D29" s="2">
-        <v>6381</v>
+        <v>156287021</v>
       </c>
       <c r="E29" s="2">
-        <v>7065</v>
+        <v>156455841</v>
       </c>
       <c r="F29" s="2">
-        <v>7321</v>
+        <v>158378456</v>
       </c>
       <c r="G29" s="2">
-        <v>9631</v>
+        <v>154612295</v>
       </c>
       <c r="H29" s="2">
-        <v>9156</v>
+        <v>158710790</v>
       </c>
       <c r="I29" s="2">
-        <v>6792</v>
+        <v>133229498</v>
       </c>
       <c r="J29" s="2">
-        <v>6729</v>
+        <v>140710087</v>
       </c>
       <c r="K29" s="2">
-        <v>1548</v>
+        <v>127690281</v>
       </c>
       <c r="L29" s="2">
-        <v>2058</v>
+        <v>132970650</v>
       </c>
       <c r="M29" s="2">
-        <v>2432</v>
+        <v>102240624</v>
       </c>
       <c r="N29" s="2">
-        <v>1933</v>
+        <v>94180287</v>
       </c>
       <c r="O29" s="2">
-        <v>309</v>
+        <v>92127247</v>
       </c>
       <c r="P29" s="2">
-        <v>95</v>
+        <v>91800049</v>
       </c>
       <c r="Q29" s="2">
-        <v>131</v>
+        <v>86765007</v>
       </c>
       <c r="R29" s="2">
-        <v>114</v>
+        <v>80038153</v>
       </c>
       <c r="S29" s="2">
-        <v>136</v>
+        <v>72154983</v>
       </c>
       <c r="T29" s="2">
-        <v>395</v>
+        <v>71866451</v>
       </c>
       <c r="U29" s="2">
-        <v>134</v>
+        <v>70992174</v>
       </c>
       <c r="V29" s="2">
-        <v>145</v>
+        <v>60914325</v>
       </c>
       <c r="W29" s="2">
-        <v>86</v>
+        <v>65444269</v>
       </c>
       <c r="X29" s="2">
-        <v>130</v>
+        <v>32765409</v>
       </c>
       <c r="Y29" s="2">
-        <v>32</v>
+        <v>4996402</v>
       </c>
       <c r="Z29" s="2">
-        <v>88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:26">
       <c r="A30" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D30" s="2">
-        <v>514137</v>
+        <v>6381</v>
       </c>
       <c r="E30" s="2">
-        <v>602491</v>
+        <v>7065</v>
       </c>
       <c r="F30" s="2">
-        <v>481344</v>
+        <v>7321</v>
       </c>
       <c r="G30" s="2">
-        <v>780815</v>
+        <v>9631</v>
       </c>
       <c r="H30" s="2">
-        <v>588317</v>
+        <v>9156</v>
       </c>
       <c r="I30" s="2">
-        <v>490084</v>
+        <v>6792</v>
       </c>
       <c r="J30" s="2">
-        <v>462417</v>
+        <v>6729</v>
       </c>
       <c r="K30" s="2">
-        <v>474550</v>
+        <v>1548</v>
       </c>
       <c r="L30" s="2">
-        <v>495363</v>
+        <v>2058</v>
       </c>
       <c r="M30" s="2">
-        <v>477112</v>
+        <v>2432</v>
       </c>
       <c r="N30" s="2">
-        <v>486864</v>
+        <v>1933</v>
       </c>
       <c r="O30" s="2">
-        <v>566104</v>
+        <v>309</v>
       </c>
       <c r="P30" s="2">
-        <v>511960</v>
+        <v>95</v>
       </c>
       <c r="Q30" s="2">
-        <v>540852</v>
+        <v>131</v>
       </c>
       <c r="R30" s="2">
-        <v>602330</v>
+        <v>114</v>
       </c>
       <c r="S30" s="2">
-        <v>603436</v>
+        <v>136</v>
       </c>
       <c r="T30" s="2">
-        <v>455811</v>
+        <v>395</v>
       </c>
       <c r="U30" s="2">
-        <v>435206</v>
+        <v>134</v>
       </c>
       <c r="V30" s="2">
-        <v>454383</v>
+        <v>145</v>
       </c>
       <c r="W30" s="2">
-        <v>555125</v>
+        <v>86</v>
       </c>
       <c r="X30" s="2">
-        <v>773966</v>
+        <v>130</v>
       </c>
       <c r="Y30" s="2">
-        <v>544708</v>
+        <v>32</v>
       </c>
       <c r="Z30" s="2">
-        <v>522878</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:26">
       <c r="A31" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D31" s="2">
-        <v>610149</v>
+        <v>514137</v>
       </c>
       <c r="E31" s="2">
-        <v>588594</v>
+        <v>602491</v>
       </c>
       <c r="F31" s="2">
-        <v>430681</v>
+        <v>481344</v>
       </c>
       <c r="G31" s="2">
-        <v>492848</v>
+        <v>780815</v>
       </c>
       <c r="H31" s="2">
-        <v>648098</v>
+        <v>588317</v>
       </c>
       <c r="I31" s="2">
-        <v>544146</v>
+        <v>490084</v>
       </c>
       <c r="J31" s="2">
-        <v>529916</v>
+        <v>462417</v>
       </c>
       <c r="K31" s="2">
-        <v>538659</v>
+        <v>474550</v>
       </c>
       <c r="L31" s="2">
-        <v>555281</v>
+        <v>495363</v>
       </c>
       <c r="M31" s="2">
-        <v>428810</v>
+        <v>477112</v>
       </c>
       <c r="N31" s="2">
-        <v>412889</v>
+        <v>486864</v>
       </c>
       <c r="O31" s="2">
-        <v>420833</v>
+        <v>566104</v>
       </c>
       <c r="P31" s="2">
-        <v>359906</v>
+        <v>511960</v>
       </c>
       <c r="Q31" s="2">
-        <v>362716</v>
+        <v>540852</v>
       </c>
       <c r="R31" s="2">
-        <v>343823</v>
+        <v>602330</v>
       </c>
       <c r="S31" s="2">
-        <v>307095</v>
+        <v>603436</v>
       </c>
       <c r="T31" s="2">
-        <v>222275</v>
+        <v>455811</v>
       </c>
       <c r="U31" s="2">
-        <v>196806</v>
+        <v>435206</v>
       </c>
       <c r="V31" s="2">
-        <v>151801</v>
+        <v>454383</v>
       </c>
       <c r="W31" s="2">
-        <v>184404</v>
+        <v>555125</v>
       </c>
       <c r="X31" s="2">
-        <v>214907</v>
+        <v>773966</v>
       </c>
       <c r="Y31" s="2">
-        <v>209715</v>
+        <v>544708</v>
       </c>
       <c r="Z31" s="2">
-        <v>154815</v>
+        <v>522878</v>
       </c>
     </row>
     <row r="32" spans="1:26">
       <c r="A32" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D32" s="2">
-        <v>212180</v>
+        <v>610149</v>
       </c>
       <c r="E32" s="2">
-        <v>655202</v>
+        <v>588594</v>
       </c>
       <c r="F32" s="2">
-        <v>1460389</v>
+        <v>430681</v>
       </c>
       <c r="G32" s="2">
-        <v>1912373</v>
+        <v>492848</v>
       </c>
       <c r="H32" s="2">
-        <v>1247656</v>
+        <v>648098</v>
       </c>
       <c r="I32" s="2">
-        <v>236987</v>
+        <v>544146</v>
       </c>
       <c r="J32" s="2">
-        <v>426545</v>
+        <v>529916</v>
       </c>
       <c r="K32" s="2">
-        <v>705991</v>
+        <v>538659</v>
       </c>
       <c r="L32" s="2">
-        <v>101015</v>
+        <v>555281</v>
       </c>
       <c r="M32" s="2">
-        <v>30594</v>
+        <v>428810</v>
       </c>
       <c r="N32" s="2">
-        <v>0</v>
+        <v>412889</v>
       </c>
       <c r="O32" s="2">
-        <v>0</v>
+        <v>420833</v>
       </c>
       <c r="P32" s="2">
-        <v>0</v>
+        <v>359906</v>
       </c>
       <c r="Q32" s="2">
-        <v>0</v>
+        <v>362716</v>
       </c>
       <c r="R32" s="2">
-        <v>0</v>
+        <v>343823</v>
       </c>
       <c r="S32" s="2">
-        <v>0</v>
+        <v>307095</v>
       </c>
       <c r="T32" s="2">
-        <v>0</v>
+        <v>222275</v>
       </c>
       <c r="U32" s="2">
-        <v>0</v>
+        <v>196806</v>
       </c>
       <c r="V32" s="2">
-        <v>0</v>
+        <v>151801</v>
       </c>
       <c r="W32" s="2">
-        <v>0</v>
+        <v>184404</v>
       </c>
       <c r="X32" s="2">
-        <v>0</v>
+        <v>214907</v>
       </c>
       <c r="Y32" s="2">
-        <v>0</v>
+        <v>209715</v>
       </c>
       <c r="Z32" s="2">
-        <v>0</v>
+        <v>154815</v>
       </c>
     </row>
     <row r="33" spans="1:26">
       <c r="A33" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D33" s="2">
-        <v>0</v>
+        <v>212180</v>
       </c>
       <c r="E33" s="2">
-        <v>0</v>
+        <v>655202</v>
       </c>
       <c r="F33" s="2">
-        <v>0</v>
+        <v>1460389</v>
       </c>
       <c r="G33" s="2">
-        <v>0</v>
+        <v>1912373</v>
       </c>
       <c r="H33" s="2">
-        <v>0</v>
+        <v>1247656</v>
       </c>
       <c r="I33" s="2">
-        <v>0</v>
+        <v>236987</v>
       </c>
       <c r="J33" s="2">
-        <v>0</v>
+        <v>426545</v>
       </c>
       <c r="K33" s="2">
-        <v>0</v>
+        <v>705991</v>
       </c>
       <c r="L33" s="2">
-        <v>0</v>
+        <v>101015</v>
       </c>
       <c r="M33" s="2">
-        <v>0</v>
+        <v>30594</v>
       </c>
       <c r="N33" s="2">
         <v>0</v>
@@ -3249,46 +3255,46 @@
     </row>
     <row r="34" spans="1:26">
       <c r="A34" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D34" s="2">
-        <v>624212</v>
+        <v>0</v>
       </c>
       <c r="E34" s="2">
-        <v>837130</v>
+        <v>0</v>
       </c>
       <c r="F34" s="2">
-        <v>954418</v>
+        <v>0</v>
       </c>
       <c r="G34" s="2">
-        <v>1118141</v>
+        <v>0</v>
       </c>
       <c r="H34" s="2">
-        <v>840672</v>
+        <v>0</v>
       </c>
       <c r="I34" s="2">
-        <v>1192742</v>
+        <v>0</v>
       </c>
       <c r="J34" s="2">
-        <v>1211524</v>
+        <v>0</v>
       </c>
       <c r="K34" s="2">
-        <v>1477066</v>
+        <v>0</v>
       </c>
       <c r="L34" s="2">
-        <v>1491182</v>
+        <v>0</v>
       </c>
       <c r="M34" s="2">
-        <v>729249</v>
+        <v>0</v>
       </c>
       <c r="N34" s="2">
-        <v>1251192</v>
+        <v>0</v>
       </c>
       <c r="O34" s="2">
         <v>0</v>
@@ -3297,25 +3303,25 @@
         <v>0</v>
       </c>
       <c r="Q34" s="2">
-        <v>42080</v>
+        <v>0</v>
       </c>
       <c r="R34" s="2">
-        <v>108742</v>
+        <v>0</v>
       </c>
       <c r="S34" s="2">
-        <v>65288</v>
+        <v>0</v>
       </c>
       <c r="T34" s="2">
-        <v>73488</v>
+        <v>0</v>
       </c>
       <c r="U34" s="2">
-        <v>85141</v>
+        <v>0</v>
       </c>
       <c r="V34" s="2">
-        <v>44447</v>
+        <v>0</v>
       </c>
       <c r="W34" s="2">
-        <v>27574</v>
+        <v>0</v>
       </c>
       <c r="X34" s="2">
         <v>0</v>
@@ -3332,43 +3338,43 @@
         <v>14</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D35" s="2">
-        <v>1804</v>
+        <v>624212</v>
       </c>
       <c r="E35" s="2">
-        <v>2790</v>
+        <v>837130</v>
       </c>
       <c r="F35" s="2">
-        <v>3033</v>
+        <v>954418</v>
       </c>
       <c r="G35" s="2">
-        <v>4759</v>
+        <v>1118141</v>
       </c>
       <c r="H35" s="2">
-        <v>5189</v>
+        <v>840672</v>
       </c>
       <c r="I35" s="2">
-        <v>5529</v>
+        <v>1192742</v>
       </c>
       <c r="J35" s="2">
-        <v>7308</v>
+        <v>1211524</v>
       </c>
       <c r="K35" s="2">
-        <v>20705</v>
+        <v>1477066</v>
       </c>
       <c r="L35" s="2">
-        <v>17437</v>
+        <v>1491182</v>
       </c>
       <c r="M35" s="2">
-        <v>0</v>
+        <v>729249</v>
       </c>
       <c r="N35" s="2">
-        <v>0</v>
+        <v>1251192</v>
       </c>
       <c r="O35" s="2">
         <v>0</v>
@@ -3377,25 +3383,25 @@
         <v>0</v>
       </c>
       <c r="Q35" s="2">
-        <v>0</v>
+        <v>42080</v>
       </c>
       <c r="R35" s="2">
-        <v>0</v>
+        <v>108742</v>
       </c>
       <c r="S35" s="2">
-        <v>0</v>
+        <v>65288</v>
       </c>
       <c r="T35" s="2">
-        <v>0</v>
+        <v>73488</v>
       </c>
       <c r="U35" s="2">
-        <v>0</v>
+        <v>85141</v>
       </c>
       <c r="V35" s="2">
-        <v>0</v>
+        <v>44447</v>
       </c>
       <c r="W35" s="2">
-        <v>0</v>
+        <v>27574</v>
       </c>
       <c r="X35" s="2">
         <v>0</v>
@@ -3409,82 +3415,82 @@
     </row>
     <row r="36" spans="1:26">
       <c r="A36" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D36" s="2">
-        <v>0</v>
+        <v>200000</v>
       </c>
       <c r="E36" s="2">
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="F36" s="2">
-        <v>0</v>
+        <v>600000</v>
       </c>
       <c r="G36" s="2">
-        <v>0</v>
+        <v>1300000</v>
       </c>
       <c r="H36" s="2">
-        <v>0</v>
+        <v>2200000</v>
       </c>
       <c r="I36" s="2">
-        <v>0</v>
+        <v>3100000</v>
       </c>
       <c r="J36" s="2">
-        <v>0</v>
+        <v>4400000</v>
       </c>
       <c r="K36" s="2">
-        <v>0</v>
+        <v>6600000</v>
       </c>
       <c r="L36" s="2">
-        <v>0</v>
+        <v>11700000</v>
       </c>
       <c r="M36" s="2">
-        <v>0</v>
+        <v>19600000</v>
       </c>
       <c r="N36" s="2">
-        <v>0</v>
+        <v>26200000</v>
       </c>
       <c r="O36" s="2">
-        <v>0</v>
+        <v>30000000</v>
       </c>
       <c r="P36" s="2">
-        <v>0</v>
+        <v>34800000</v>
       </c>
       <c r="Q36" s="2">
-        <v>0</v>
+        <v>37300000</v>
       </c>
       <c r="R36" s="2">
-        <v>0</v>
+        <v>36800000</v>
       </c>
       <c r="S36" s="2">
-        <v>0</v>
+        <v>38000000</v>
       </c>
       <c r="T36" s="2">
-        <v>0</v>
+        <v>43500000</v>
       </c>
       <c r="U36" s="2">
-        <v>0</v>
+        <v>44300000</v>
       </c>
       <c r="V36" s="2">
-        <v>0</v>
+        <v>48500000</v>
       </c>
       <c r="W36" s="2">
-        <v>0</v>
+        <v>48400000</v>
       </c>
       <c r="X36" s="2">
-        <v>0</v>
+        <v>60300000</v>
       </c>
       <c r="Y36" s="2">
-        <v>0</v>
+        <v>61100000</v>
       </c>
       <c r="Z36" s="2">
-        <v>0</v>
+        <v>74100000</v>
       </c>
     </row>
     <row r="37" spans="1:26">
@@ -3492,10 +3498,10 @@
         <v>15</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D37" s="2">
         <v>0</v>
@@ -3546,10 +3552,10 @@
         <v>0</v>
       </c>
       <c r="T37" s="2">
-        <v>73797</v>
+        <v>0</v>
       </c>
       <c r="U37" s="2">
-        <v>21676</v>
+        <v>0</v>
       </c>
       <c r="V37" s="2">
         <v>0</v>
@@ -3569,46 +3575,46 @@
     </row>
     <row r="38" spans="1:26">
       <c r="A38" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D38" s="2">
-        <v>23853</v>
+        <v>0</v>
       </c>
       <c r="E38" s="2">
-        <v>586925</v>
+        <v>0</v>
       </c>
       <c r="F38" s="2">
-        <v>476303</v>
+        <v>0</v>
       </c>
       <c r="G38" s="2">
-        <v>461587</v>
+        <v>0</v>
       </c>
       <c r="H38" s="2">
-        <v>541038</v>
+        <v>0</v>
       </c>
       <c r="I38" s="2">
-        <v>496684</v>
+        <v>0</v>
       </c>
       <c r="J38" s="2">
-        <v>526695</v>
+        <v>0</v>
       </c>
       <c r="K38" s="2">
-        <v>507018</v>
+        <v>0</v>
       </c>
       <c r="L38" s="2">
-        <v>487452</v>
+        <v>0</v>
       </c>
       <c r="M38" s="2">
-        <v>240326</v>
+        <v>0</v>
       </c>
       <c r="N38" s="2">
-        <v>215849</v>
+        <v>0</v>
       </c>
       <c r="O38" s="2">
         <v>0</v>
@@ -3617,19 +3623,19 @@
         <v>0</v>
       </c>
       <c r="Q38" s="2">
-        <v>30406</v>
+        <v>0</v>
       </c>
       <c r="R38" s="2">
-        <v>44992</v>
+        <v>0</v>
       </c>
       <c r="S38" s="2">
-        <v>41829</v>
+        <v>0</v>
       </c>
       <c r="T38" s="2">
-        <v>0</v>
+        <v>73797</v>
       </c>
       <c r="U38" s="2">
-        <v>0</v>
+        <v>21676</v>
       </c>
       <c r="V38" s="2">
         <v>0</v>
@@ -3649,46 +3655,46 @@
     </row>
     <row r="39" spans="1:26">
       <c r="A39" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D39" s="2">
-        <v>0</v>
+        <v>23853</v>
       </c>
       <c r="E39" s="2">
-        <v>0</v>
+        <v>586925</v>
       </c>
       <c r="F39" s="2">
-        <v>0</v>
+        <v>476303</v>
       </c>
       <c r="G39" s="2">
-        <v>0</v>
+        <v>461587</v>
       </c>
       <c r="H39" s="2">
-        <v>0</v>
+        <v>541038</v>
       </c>
       <c r="I39" s="2">
-        <v>0</v>
+        <v>496684</v>
       </c>
       <c r="J39" s="2">
-        <v>0</v>
+        <v>526695</v>
       </c>
       <c r="K39" s="2">
-        <v>0</v>
+        <v>507018</v>
       </c>
       <c r="L39" s="2">
-        <v>0</v>
+        <v>487452</v>
       </c>
       <c r="M39" s="2">
-        <v>0</v>
+        <v>240326</v>
       </c>
       <c r="N39" s="2">
-        <v>0</v>
+        <v>215849</v>
       </c>
       <c r="O39" s="2">
         <v>0</v>
@@ -3697,13 +3703,13 @@
         <v>0</v>
       </c>
       <c r="Q39" s="2">
-        <v>0</v>
+        <v>30406</v>
       </c>
       <c r="R39" s="2">
-        <v>0</v>
+        <v>44992</v>
       </c>
       <c r="S39" s="2">
-        <v>0</v>
+        <v>41829</v>
       </c>
       <c r="T39" s="2">
         <v>0</v>
@@ -3729,13 +3735,13 @@
     </row>
     <row r="40" spans="1:26">
       <c r="A40" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D40" s="2">
         <v>0</v>
@@ -3792,16 +3798,16 @@
         <v>0</v>
       </c>
       <c r="V40" s="2">
-        <v>4912</v>
+        <v>0</v>
       </c>
       <c r="W40" s="2">
-        <v>3880</v>
+        <v>0</v>
       </c>
       <c r="X40" s="2">
         <v>0</v>
       </c>
       <c r="Y40" s="2">
-        <v>1227</v>
+        <v>0</v>
       </c>
       <c r="Z40" s="2">
         <v>0</v>
@@ -3809,13 +3815,13 @@
     </row>
     <row r="41" spans="1:26">
       <c r="A41" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D41" s="2">
         <v>0</v>
@@ -3889,13 +3895,13 @@
     </row>
     <row r="42" spans="1:26">
       <c r="A42" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D42" s="2">
         <v>0</v>
@@ -3969,13 +3975,13 @@
     </row>
     <row r="43" spans="1:26">
       <c r="A43" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D43" s="2">
         <v>0</v>
@@ -4049,13 +4055,13 @@
     </row>
     <row r="44" spans="1:26">
       <c r="A44" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D44" s="2">
         <v>441932</v>
@@ -4129,13 +4135,13 @@
     </row>
     <row r="45" spans="1:26">
       <c r="A45" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D45" s="2">
         <v>111426567</v>
@@ -4209,13 +4215,13 @@
     </row>
     <row r="46" spans="1:26">
       <c r="A46" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D46" s="2">
         <v>0</v>
@@ -4289,13 +4295,13 @@
     </row>
     <row r="47" spans="1:26">
       <c r="A47" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D47" s="2">
         <v>0</v>
@@ -4369,13 +4375,13 @@
     </row>
     <row r="48" spans="1:26">
       <c r="A48" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D48" s="2">
         <v>0</v>
@@ -4449,13 +4455,13 @@
     </row>
     <row r="49" spans="1:26">
       <c r="A49" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D49" s="2">
         <v>17987251</v>
@@ -4529,13 +4535,13 @@
     </row>
     <row r="50" spans="1:26">
       <c r="A50" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D50" s="2">
         <v>0</v>
@@ -4609,13 +4615,13 @@
     </row>
     <row r="51" spans="1:26">
       <c r="A51" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D51" s="2">
         <v>0</v>
@@ -4689,13 +4695,13 @@
     </row>
     <row r="52" spans="1:26">
       <c r="A52" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D52" s="2">
         <v>3933611</v>
@@ -4769,13 +4775,13 @@
     </row>
     <row r="53" spans="1:26">
       <c r="A53" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D53" s="2">
         <v>2060394</v>
@@ -4849,40 +4855,40 @@
     </row>
     <row r="54" spans="1:26">
       <c r="A54" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D54" s="2">
-        <v>156818</v>
+        <v>0</v>
       </c>
       <c r="E54" s="2">
-        <v>167254</v>
+        <v>0</v>
       </c>
       <c r="F54" s="2">
-        <v>287558</v>
+        <v>0</v>
       </c>
       <c r="G54" s="2">
-        <v>308215</v>
+        <v>0</v>
       </c>
       <c r="H54" s="2">
-        <v>340179</v>
+        <v>0</v>
       </c>
       <c r="I54" s="2">
-        <v>442074</v>
+        <v>0</v>
       </c>
       <c r="J54" s="2">
-        <v>459919</v>
+        <v>0</v>
       </c>
       <c r="K54" s="2">
-        <v>448287</v>
+        <v>0</v>
       </c>
       <c r="L54" s="2">
-        <v>419334</v>
+        <v>0</v>
       </c>
       <c r="M54" s="2">
         <v>0</v>
@@ -4912,19 +4918,99 @@
         <v>0</v>
       </c>
       <c r="V54" s="2">
-        <v>0</v>
+        <v>4912</v>
       </c>
       <c r="W54" s="2">
-        <v>0</v>
+        <v>3880</v>
       </c>
       <c r="X54" s="2">
         <v>0</v>
       </c>
       <c r="Y54" s="2">
-        <v>0</v>
+        <v>1227</v>
       </c>
       <c r="Z54" s="2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26">
+      <c r="A55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" s="2">
+        <v>15500000</v>
+      </c>
+      <c r="E55" s="2">
+        <v>18700000</v>
+      </c>
+      <c r="F55" s="2">
+        <v>25500000</v>
+      </c>
+      <c r="G55" s="2">
+        <v>27200000</v>
+      </c>
+      <c r="H55" s="2">
+        <v>30700000</v>
+      </c>
+      <c r="I55" s="2">
+        <v>39700000</v>
+      </c>
+      <c r="J55" s="2">
+        <v>40600000</v>
+      </c>
+      <c r="K55" s="2">
+        <v>38600000</v>
+      </c>
+      <c r="L55" s="2">
+        <v>39800000</v>
+      </c>
+      <c r="M55" s="2">
+        <v>48900000</v>
+      </c>
+      <c r="N55" s="2">
+        <v>50600000</v>
+      </c>
+      <c r="O55" s="2">
+        <v>51700000</v>
+      </c>
+      <c r="P55" s="2">
+        <v>57300000</v>
+      </c>
+      <c r="Q55" s="2">
+        <v>79100000</v>
+      </c>
+      <c r="R55" s="2">
+        <v>78400000</v>
+      </c>
+      <c r="S55" s="2">
+        <v>103700000</v>
+      </c>
+      <c r="T55" s="2">
+        <v>107900000</v>
+      </c>
+      <c r="U55" s="2">
+        <v>123600000</v>
+      </c>
+      <c r="V55" s="2">
+        <v>129600000</v>
+      </c>
+      <c r="W55" s="2">
+        <v>112500000</v>
+      </c>
+      <c r="X55" s="2">
+        <v>124800000</v>
+      </c>
+      <c r="Y55" s="2">
+        <v>137800000</v>
+      </c>
+      <c r="Z55" s="2">
+        <v>138900000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>